<commit_message>
Highligh review title and JavaScript changes
</commit_message>
<xml_diff>
--- a/MobileAppReviews/uploaded_files/ReviewMiner/Review_Criteria.xlsx
+++ b/MobileAppReviews/uploaded_files/ReviewMiner/Review_Criteria.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viral\PycharmProjects\Technical-AppReviews\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viral\PycharmProjects\Technical-AppReviews\MobileAppReviews\uploaded_files\ReviewMiner\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>word</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>flaw</t>
-  </si>
-  <si>
-    <t>poor</t>
   </si>
   <si>
     <t>useless</t>
@@ -232,12 +229,6 @@
     <t>frustrate</t>
   </si>
   <si>
-    <t>doesn't</t>
-  </si>
-  <si>
-    <t>don't</t>
-  </si>
-  <si>
     <t>block</t>
   </si>
   <si>
@@ -284,6 +275,36 @@
   </si>
   <si>
     <t>please allow</t>
+  </si>
+  <si>
+    <t>doesn’t</t>
+  </si>
+  <si>
+    <t>don’t</t>
+  </si>
+  <si>
+    <t>dont</t>
+  </si>
+  <si>
+    <t>doesnt</t>
+  </si>
+  <si>
+    <t>not working</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>can't</t>
+  </si>
+  <si>
+    <t>cant</t>
+  </si>
+  <si>
+    <t>please fix</t>
+  </si>
+  <si>
+    <t>interface</t>
   </si>
 </sst>
 </file>
@@ -657,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -891,18 +912,10 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25">
-        <f>SUM(B2:B24)</f>
-        <v>78</v>
+      <c r="A24" s="5"/>
+      <c r="B24">
+        <f>SUM(B2:B23)</f>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -912,9 +925,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="A7:XFD7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -923,10 +938,10 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -955,7 +970,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="6">
         <v>3</v>
@@ -987,7 +1002,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6">
         <v>3</v>
@@ -1019,7 +1034,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6">
         <v>3</v>
@@ -1051,7 +1066,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="6">
         <v>4</v>
@@ -1083,7 +1098,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6">
         <v>3</v>
@@ -1114,8 +1129,8 @@
       <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>32</v>
+      <c r="A7" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B7" s="6">
         <v>4</v>
@@ -1146,8 +1161,8 @@
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>33</v>
+      <c r="A8" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="B8" s="6">
         <v>4</v>
@@ -1179,7 +1194,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6">
         <v>4</v>
@@ -1210,15 +1225,13 @@
       <c r="Z9" s="7"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>35</v>
+      <c r="A10" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="B10" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1244,12 +1257,15 @@
       <c r="Z10" s="7"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7">
-        <f>SUM(B2:B10)</f>
-        <v>31</v>
+      <c r="A11" s="8" t="s">
+        <v>34</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="B11" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1276,7 +1292,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
+      <c r="B12" s="7">
+        <f>SUM(B2:B11)</f>
+        <v>35</v>
+      </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1470,7 +1489,7 @@
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
     </row>
-    <row r="19" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -28966,6 +28985,34 @@
       <c r="Y1000" s="7"/>
       <c r="Z1000" s="7"/>
     </row>
+    <row r="1001" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A1001" s="7"/>
+      <c r="B1001" s="7"/>
+      <c r="C1001" s="7"/>
+      <c r="D1001" s="7"/>
+      <c r="E1001" s="7"/>
+      <c r="F1001" s="7"/>
+      <c r="G1001" s="7"/>
+      <c r="H1001" s="7"/>
+      <c r="I1001" s="7"/>
+      <c r="J1001" s="7"/>
+      <c r="K1001" s="7"/>
+      <c r="L1001" s="7"/>
+      <c r="M1001" s="7"/>
+      <c r="N1001" s="7"/>
+      <c r="O1001" s="7"/>
+      <c r="P1001" s="7"/>
+      <c r="Q1001" s="7"/>
+      <c r="R1001" s="7"/>
+      <c r="S1001" s="7"/>
+      <c r="T1001" s="7"/>
+      <c r="U1001" s="7"/>
+      <c r="V1001" s="7"/>
+      <c r="W1001" s="7"/>
+      <c r="X1001" s="7"/>
+      <c r="Y1001" s="7"/>
+      <c r="Z1001" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28975,21 +29022,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3">
         <v>4</v>
@@ -28997,7 +29046,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -29005,7 +29054,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3">
         <v>5</v>
@@ -29024,25 +29073,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3">
         <v>3</v>
@@ -29050,7 +29099,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -29058,7 +29107,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3">
         <v>4</v>
@@ -29066,7 +29115,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
@@ -29074,7 +29123,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -29082,7 +29131,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -29090,7 +29139,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -29098,7 +29147,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
@@ -29106,7 +29155,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -29114,7 +29163,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -29122,7 +29171,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -29130,24 +29179,32 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>55</v>
+      <c r="A14" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="B14" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <f>SUM(B2:B14)</f>
-        <v>40</v>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f>SUM(B2:B15)</f>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -29157,33 +29214,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>58</v>
+      <c r="A2" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="B2" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="6">
         <v>3</v>
@@ -29191,7 +29248,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="6">
         <v>2</v>
@@ -29199,7 +29256,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
@@ -29207,7 +29264,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="6">
         <v>3</v>
@@ -29215,7 +29272,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
@@ -29223,7 +29280,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="6">
         <v>2</v>
@@ -29231,7 +29288,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B9" s="6">
         <v>3</v>
@@ -29239,7 +29296,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="6">
         <v>3</v>
@@ -29247,7 +29304,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="6">
         <v>2</v>
@@ -29255,7 +29312,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="6">
         <v>4</v>
@@ -29263,15 +29320,15 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B13" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B14" s="6">
         <v>3</v>
@@ -29279,71 +29336,71 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B15" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B16" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="6">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="6">
+      <c r="B22" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="6">
-        <v>4</v>
-      </c>
-    </row>
     <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B23" s="6">
         <v>2</v>
@@ -29351,7 +29408,7 @@
     </row>
     <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B24" s="6">
         <v>4</v>
@@ -29359,48 +29416,96 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="6">
-        <v>4</v>
+      <c r="B30" s="6">
+        <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+    <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B27" s="6">
+      <c r="B35" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B30">
-        <f>SUM(B2:B29)</f>
-        <v>76</v>
+    <row r="36" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <f>SUM(B2:B35)</f>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more screenshots added for report
</commit_message>
<xml_diff>
--- a/MobileAppReviews/uploaded_files/ReviewMiner/Review_Criteria.xlsx
+++ b/MobileAppReviews/uploaded_files/ReviewMiner/Review_Criteria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -680,9 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -927,7 +925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Blog added in ReadMe file
</commit_message>
<xml_diff>
--- a/MobileAppReviews/uploaded_files/ReviewMiner/Review_Criteria.xlsx
+++ b/MobileAppReviews/uploaded_files/ReviewMiner/Review_Criteria.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>ads</t>
-  </si>
-  <si>
-    <t>advertisement</t>
   </si>
   <si>
     <t>promotion</t>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>interface</t>
+  </si>
+  <si>
+    <t>advertisements</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="B3" s="6">
         <v>3</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="6">
         <v>3</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="6">
         <v>4</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="6">
         <v>3</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="6">
         <v>4</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="6">
         <v>4</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="6">
         <v>4</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6">
         <v>4</v>
@@ -1256,13 +1256,13 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6">
         <v>3</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -29028,15 +29028,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="3">
         <v>4</v>
@@ -29044,7 +29044,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -29052,7 +29052,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3">
         <v>5</v>
@@ -29081,15 +29081,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B2" s="3">
         <v>3</v>
@@ -29097,7 +29097,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -29105,7 +29105,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3">
         <v>4</v>
@@ -29113,7 +29113,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
@@ -29121,7 +29121,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -29129,7 +29129,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -29137,7 +29137,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -29145,7 +29145,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
@@ -29153,7 +29153,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
@@ -29161,7 +29161,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -29169,7 +29169,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
@@ -29177,7 +29177,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="3">
         <v>2</v>
@@ -29185,7 +29185,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
@@ -29193,7 +29193,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B15" s="3">
         <v>3</v>
@@ -29222,15 +29222,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="6">
         <v>3</v>
@@ -29238,7 +29238,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="6">
         <v>3</v>
@@ -29246,7 +29246,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="6">
         <v>2</v>
@@ -29254,7 +29254,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="6">
         <v>3</v>
@@ -29262,7 +29262,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="6">
         <v>3</v>
@@ -29270,7 +29270,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="6">
         <v>3</v>
@@ -29278,7 +29278,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="6">
         <v>2</v>
@@ -29286,7 +29286,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="6">
         <v>3</v>
@@ -29294,7 +29294,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="6">
         <v>3</v>
@@ -29302,7 +29302,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="6">
         <v>2</v>
@@ -29310,7 +29310,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="6">
         <v>4</v>
@@ -29318,7 +29318,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="6">
         <v>2</v>
@@ -29326,7 +29326,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" s="6">
         <v>3</v>
@@ -29334,7 +29334,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="6">
         <v>3</v>
@@ -29342,7 +29342,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="6">
         <v>3</v>
@@ -29350,7 +29350,7 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" s="6">
         <v>4</v>
@@ -29358,7 +29358,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="6">
         <v>3</v>
@@ -29366,7 +29366,7 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" s="6">
         <v>-2</v>
@@ -29374,7 +29374,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="6">
         <v>4</v>
@@ -29382,7 +29382,7 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" s="6">
         <v>3</v>
@@ -29390,7 +29390,7 @@
     </row>
     <row r="22" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="6">
         <v>3</v>
@@ -29398,7 +29398,7 @@
     </row>
     <row r="23" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B23" s="6">
         <v>2</v>
@@ -29406,7 +29406,7 @@
     </row>
     <row r="24" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="6">
         <v>4</v>
@@ -29414,7 +29414,7 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="6">
         <v>2</v>
@@ -29422,7 +29422,7 @@
     </row>
     <row r="26" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" s="6">
         <v>4</v>
@@ -29430,7 +29430,7 @@
     </row>
     <row r="27" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="6">
         <v>4</v>
@@ -29438,7 +29438,7 @@
     </row>
     <row r="28" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" s="6">
         <v>3</v>
@@ -29446,7 +29446,7 @@
     </row>
     <row r="29" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" s="6">
         <v>2</v>
@@ -29454,7 +29454,7 @@
     </row>
     <row r="30" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" s="6">
         <v>2</v>
@@ -29462,7 +29462,7 @@
     </row>
     <row r="31" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="6">
         <v>2</v>
@@ -29470,7 +29470,7 @@
     </row>
     <row r="32" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" s="6">
         <v>2</v>
@@ -29478,7 +29478,7 @@
     </row>
     <row r="33" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" s="6">
         <v>3</v>
@@ -29486,7 +29486,7 @@
     </row>
     <row r="34" spans="1:2" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" s="6">
         <v>3</v>
@@ -29494,7 +29494,7 @@
     </row>
     <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="3">
         <v>2</v>

</xml_diff>